<commit_message>
adding count var for testing
</commit_message>
<xml_diff>
--- a/responses.xlsx
+++ b/responses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshvasilvasstar/Documents/clinicchat/dh-c4h-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A7CE34-A44F-5747-A9C0-F07D54E447A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{064BEC13-2A17-CC41-B368-559FF77FEAF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="7580" windowWidth="27640" windowHeight="16940" xr2:uid="{E7C9F955-17B0-F040-8EA4-EA009C6A7680}"/>
+    <workbookView xWindow="5900" yWindow="9820" windowWidth="27640" windowHeight="16940" xr2:uid="{E7C9F955-17B0-F040-8EA4-EA009C6A7680}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2566" uniqueCount="1186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2566" uniqueCount="1187">
   <si>
     <t>Why should I eat healthy food?</t>
   </si>
@@ -4033,6 +4033,9 @@
   </si>
   <si>
     <t>En Denver Health, después de haber recibido sus recetas por correo por primera vez, puede ordenar recargas llamando a la línea de recarga automatizada al 303-389-1390, a través del sitio web de MyChart o a través de la aplicación de teléfonos inteligentes MyChart. Las recargas no se envían automáticamente.</t>
+  </si>
+  <si>
+    <t>Quit Tobacco</t>
   </si>
 </sst>
 </file>
@@ -4582,11 +4585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC232BA-84F4-BE49-B367-4C71587DA4B6}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:H219"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C224" sqref="C224"/>
+      <selection activeCell="A154" sqref="A154:A164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4622,7 +4624,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1">
+    <row r="2" spans="1:8">
       <c r="A2" s="8" t="s">
         <v>384</v>
       </c>
@@ -4648,7 +4650,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1">
+    <row r="3" spans="1:8">
       <c r="A3" s="8" t="s">
         <v>384</v>
       </c>
@@ -4674,7 +4676,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1">
+    <row r="4" spans="1:8">
       <c r="A4" s="8" t="s">
         <v>391</v>
       </c>
@@ -4700,7 +4702,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1">
+    <row r="5" spans="1:8">
       <c r="A5" s="8" t="s">
         <v>391</v>
       </c>
@@ -4726,7 +4728,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1">
+    <row r="6" spans="1:8">
       <c r="A6" s="8" t="s">
         <v>391</v>
       </c>
@@ -4752,7 +4754,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1">
+    <row r="7" spans="1:8">
       <c r="A7" s="8" t="s">
         <v>391</v>
       </c>
@@ -4778,7 +4780,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1">
+    <row r="8" spans="1:8">
       <c r="A8" s="8" t="s">
         <v>391</v>
       </c>
@@ -4804,7 +4806,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1">
+    <row r="9" spans="1:8">
       <c r="A9" s="8" t="s">
         <v>391</v>
       </c>
@@ -4830,7 +4832,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1">
+    <row r="10" spans="1:8">
       <c r="A10" s="8" t="s">
         <v>391</v>
       </c>
@@ -4856,7 +4858,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1">
+    <row r="11" spans="1:8">
       <c r="A11" s="8" t="s">
         <v>383</v>
       </c>
@@ -4882,7 +4884,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1">
+    <row r="12" spans="1:8">
       <c r="A12" s="8" t="s">
         <v>383</v>
       </c>
@@ -4908,7 +4910,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1">
+    <row r="13" spans="1:8">
       <c r="A13" s="8" t="s">
         <v>383</v>
       </c>
@@ -4934,7 +4936,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1">
+    <row r="14" spans="1:8">
       <c r="A14" s="8" t="s">
         <v>383</v>
       </c>
@@ -4960,7 +4962,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1">
+    <row r="15" spans="1:8">
       <c r="A15" s="8" t="s">
         <v>383</v>
       </c>
@@ -4986,7 +4988,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1">
+    <row r="16" spans="1:8">
       <c r="A16" s="8" t="s">
         <v>383</v>
       </c>
@@ -5012,7 +5014,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1">
+    <row r="17" spans="1:8">
       <c r="A17" s="8" t="s">
         <v>383</v>
       </c>
@@ -5038,7 +5040,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1">
+    <row r="18" spans="1:8">
       <c r="A18" s="8" t="s">
         <v>383</v>
       </c>
@@ -5064,7 +5066,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="19" spans="1:8" hidden="1">
+    <row r="19" spans="1:8">
       <c r="A19" s="8" t="s">
         <v>383</v>
       </c>
@@ -5090,7 +5092,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="20" spans="1:8" hidden="1">
+    <row r="20" spans="1:8">
       <c r="A20" s="8" t="s">
         <v>383</v>
       </c>
@@ -5116,7 +5118,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="21" spans="1:8" hidden="1">
+    <row r="21" spans="1:8">
       <c r="A21" s="8" t="s">
         <v>383</v>
       </c>
@@ -5142,7 +5144,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="22" spans="1:8" hidden="1">
+    <row r="22" spans="1:8">
       <c r="A22" s="8" t="s">
         <v>383</v>
       </c>
@@ -5168,7 +5170,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1">
+    <row r="23" spans="1:8">
       <c r="A23" s="8" t="s">
         <v>383</v>
       </c>
@@ -5194,7 +5196,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1">
+    <row r="24" spans="1:8">
       <c r="A24" s="8" t="s">
         <v>383</v>
       </c>
@@ -5220,7 +5222,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="25" spans="1:8" hidden="1">
+    <row r="25" spans="1:8">
       <c r="A25" s="8" t="s">
         <v>383</v>
       </c>
@@ -5246,7 +5248,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="26" spans="1:8" hidden="1">
+    <row r="26" spans="1:8">
       <c r="A26" s="8" t="s">
         <v>383</v>
       </c>
@@ -5272,7 +5274,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="27" spans="1:8" hidden="1">
+    <row r="27" spans="1:8">
       <c r="A27" s="8" t="s">
         <v>383</v>
       </c>
@@ -5298,7 +5300,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="28" spans="1:8" hidden="1">
+    <row r="28" spans="1:8">
       <c r="A28" s="8" t="s">
         <v>383</v>
       </c>
@@ -5324,7 +5326,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="29" spans="1:8" hidden="1">
+    <row r="29" spans="1:8">
       <c r="A29" s="8" t="s">
         <v>383</v>
       </c>
@@ -5350,7 +5352,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="30" spans="1:8" hidden="1">
+    <row r="30" spans="1:8">
       <c r="A30" s="8" t="s">
         <v>384</v>
       </c>
@@ -5376,7 +5378,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="31" spans="1:8" hidden="1">
+    <row r="31" spans="1:8">
       <c r="A31" s="8" t="s">
         <v>384</v>
       </c>
@@ -5402,7 +5404,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="32" spans="1:8" hidden="1">
+    <row r="32" spans="1:8">
       <c r="A32" s="8" t="s">
         <v>384</v>
       </c>
@@ -5428,7 +5430,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="33" spans="1:8" hidden="1">
+    <row r="33" spans="1:8">
       <c r="A33" s="8" t="s">
         <v>384</v>
       </c>
@@ -5454,7 +5456,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="34" spans="1:8" hidden="1">
+    <row r="34" spans="1:8">
       <c r="A34" s="8" t="s">
         <v>384</v>
       </c>
@@ -5480,7 +5482,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="35" spans="1:8" hidden="1">
+    <row r="35" spans="1:8">
       <c r="A35" s="8" t="s">
         <v>384</v>
       </c>
@@ -5506,7 +5508,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="36" spans="1:8" hidden="1">
+    <row r="36" spans="1:8">
       <c r="A36" s="8" t="s">
         <v>384</v>
       </c>
@@ -5532,7 +5534,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="37" spans="1:8" hidden="1">
+    <row r="37" spans="1:8">
       <c r="A37" s="8" t="s">
         <v>384</v>
       </c>
@@ -5558,7 +5560,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="38" spans="1:8" hidden="1">
+    <row r="38" spans="1:8">
       <c r="A38" s="8" t="s">
         <v>384</v>
       </c>
@@ -5584,7 +5586,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="39" spans="1:8" hidden="1">
+    <row r="39" spans="1:8">
       <c r="A39" s="8" t="s">
         <v>384</v>
       </c>
@@ -5610,7 +5612,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="40" spans="1:8" hidden="1">
+    <row r="40" spans="1:8">
       <c r="A40" s="8" t="s">
         <v>384</v>
       </c>
@@ -5636,7 +5638,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="41" spans="1:8" hidden="1">
+    <row r="41" spans="1:8">
       <c r="A41" s="8" t="s">
         <v>384</v>
       </c>
@@ -5662,7 +5664,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="42" spans="1:8" hidden="1">
+    <row r="42" spans="1:8">
       <c r="A42" s="8" t="s">
         <v>384</v>
       </c>
@@ -5688,7 +5690,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="43" spans="1:8" hidden="1">
+    <row r="43" spans="1:8">
       <c r="A43" s="8" t="s">
         <v>384</v>
       </c>
@@ -5714,7 +5716,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="44" spans="1:8" hidden="1">
+    <row r="44" spans="1:8">
       <c r="A44" s="8" t="s">
         <v>384</v>
       </c>
@@ -5740,7 +5742,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="45" spans="1:8" hidden="1">
+    <row r="45" spans="1:8">
       <c r="A45" s="8" t="s">
         <v>384</v>
       </c>
@@ -5766,7 +5768,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="46" spans="1:8" hidden="1">
+    <row r="46" spans="1:8">
       <c r="A46" s="8" t="s">
         <v>384</v>
       </c>
@@ -5792,7 +5794,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="47" spans="1:8" hidden="1">
+    <row r="47" spans="1:8">
       <c r="A47" s="8" t="s">
         <v>384</v>
       </c>
@@ -5818,7 +5820,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="48" spans="1:8" hidden="1">
+    <row r="48" spans="1:8">
       <c r="A48" s="8" t="s">
         <v>384</v>
       </c>
@@ -5844,7 +5846,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="49" spans="1:8" hidden="1">
+    <row r="49" spans="1:8">
       <c r="A49" s="8" t="s">
         <v>384</v>
       </c>
@@ -5870,7 +5872,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="50" spans="1:8" hidden="1">
+    <row r="50" spans="1:8">
       <c r="A50" s="8" t="s">
         <v>384</v>
       </c>
@@ -5896,7 +5898,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="51" spans="1:8" hidden="1">
+    <row r="51" spans="1:8">
       <c r="A51" s="8" t="s">
         <v>384</v>
       </c>
@@ -5922,7 +5924,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="52" spans="1:8" hidden="1">
+    <row r="52" spans="1:8">
       <c r="A52" s="8" t="s">
         <v>384</v>
       </c>
@@ -5948,7 +5950,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="53" spans="1:8" hidden="1">
+    <row r="53" spans="1:8">
       <c r="A53" s="8" t="s">
         <v>384</v>
       </c>
@@ -5974,7 +5976,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="54" spans="1:8" hidden="1">
+    <row r="54" spans="1:8">
       <c r="A54" s="8" t="s">
         <v>384</v>
       </c>
@@ -6000,7 +6002,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="55" spans="1:8" hidden="1">
+    <row r="55" spans="1:8">
       <c r="A55" s="8" t="s">
         <v>384</v>
       </c>
@@ -6026,7 +6028,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="56" spans="1:8" hidden="1">
+    <row r="56" spans="1:8">
       <c r="A56" s="8" t="s">
         <v>384</v>
       </c>
@@ -6052,7 +6054,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="57" spans="1:8" hidden="1">
+    <row r="57" spans="1:8">
       <c r="A57" s="8" t="s">
         <v>384</v>
       </c>
@@ -6078,7 +6080,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="58" spans="1:8" hidden="1">
+    <row r="58" spans="1:8">
       <c r="A58" s="8" t="s">
         <v>384</v>
       </c>
@@ -6104,7 +6106,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="59" spans="1:8" hidden="1">
+    <row r="59" spans="1:8">
       <c r="A59" s="8" t="s">
         <v>385</v>
       </c>
@@ -6130,7 +6132,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="60" spans="1:8" hidden="1">
+    <row r="60" spans="1:8">
       <c r="A60" s="8" t="s">
         <v>385</v>
       </c>
@@ -6156,7 +6158,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="61" spans="1:8" hidden="1">
+    <row r="61" spans="1:8">
       <c r="A61" s="8" t="s">
         <v>385</v>
       </c>
@@ -6182,7 +6184,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="62" spans="1:8" hidden="1">
+    <row r="62" spans="1:8">
       <c r="A62" s="8" t="s">
         <v>385</v>
       </c>
@@ -6208,7 +6210,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="63" spans="1:8" hidden="1">
+    <row r="63" spans="1:8">
       <c r="A63" s="8" t="s">
         <v>385</v>
       </c>
@@ -6234,7 +6236,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="64" spans="1:8" hidden="1">
+    <row r="64" spans="1:8">
       <c r="A64" s="8" t="s">
         <v>385</v>
       </c>
@@ -6260,7 +6262,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="65" spans="1:8" hidden="1">
+    <row r="65" spans="1:8">
       <c r="A65" s="8" t="s">
         <v>385</v>
       </c>
@@ -6286,7 +6288,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="66" spans="1:8" hidden="1">
+    <row r="66" spans="1:8">
       <c r="A66" s="8" t="s">
         <v>385</v>
       </c>
@@ -6312,7 +6314,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="67" spans="1:8" hidden="1">
+    <row r="67" spans="1:8">
       <c r="A67" s="8" t="s">
         <v>386</v>
       </c>
@@ -6338,7 +6340,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="68" spans="1:8" hidden="1">
+    <row r="68" spans="1:8">
       <c r="A68" s="8" t="s">
         <v>386</v>
       </c>
@@ -6364,7 +6366,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="69" spans="1:8" hidden="1">
+    <row r="69" spans="1:8">
       <c r="A69" s="8" t="s">
         <v>386</v>
       </c>
@@ -6390,7 +6392,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="70" spans="1:8" hidden="1">
+    <row r="70" spans="1:8">
       <c r="A70" s="8" t="s">
         <v>386</v>
       </c>
@@ -6416,7 +6418,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="71" spans="1:8" hidden="1">
+    <row r="71" spans="1:8">
       <c r="A71" s="8" t="s">
         <v>386</v>
       </c>
@@ -6442,7 +6444,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="72" spans="1:8" hidden="1">
+    <row r="72" spans="1:8">
       <c r="A72" s="8" t="s">
         <v>386</v>
       </c>
@@ -6468,7 +6470,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="73" spans="1:8" hidden="1">
+    <row r="73" spans="1:8">
       <c r="A73" s="8" t="s">
         <v>386</v>
       </c>
@@ -6494,7 +6496,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="74" spans="1:8" hidden="1">
+    <row r="74" spans="1:8">
       <c r="A74" s="8" t="s">
         <v>386</v>
       </c>
@@ -6520,7 +6522,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="75" spans="1:8" hidden="1">
+    <row r="75" spans="1:8">
       <c r="A75" s="8" t="s">
         <v>386</v>
       </c>
@@ -6546,7 +6548,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="76" spans="1:8" hidden="1">
+    <row r="76" spans="1:8">
       <c r="A76" s="8" t="s">
         <v>386</v>
       </c>
@@ -6572,7 +6574,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="77" spans="1:8" hidden="1">
+    <row r="77" spans="1:8">
       <c r="A77" s="8" t="s">
         <v>386</v>
       </c>
@@ -6598,7 +6600,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="78" spans="1:8" hidden="1">
+    <row r="78" spans="1:8">
       <c r="A78" s="8" t="s">
         <v>386</v>
       </c>
@@ -6624,7 +6626,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="79" spans="1:8" hidden="1">
+    <row r="79" spans="1:8">
       <c r="A79" s="8" t="s">
         <v>387</v>
       </c>
@@ -6650,7 +6652,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="80" spans="1:8" hidden="1">
+    <row r="80" spans="1:8">
       <c r="A80" s="8" t="s">
         <v>387</v>
       </c>
@@ -6676,7 +6678,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="81" spans="1:8" hidden="1">
+    <row r="81" spans="1:8">
       <c r="A81" s="8" t="s">
         <v>387</v>
       </c>
@@ -6702,7 +6704,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="82" spans="1:8" hidden="1">
+    <row r="82" spans="1:8">
       <c r="A82" s="8" t="s">
         <v>387</v>
       </c>
@@ -6728,7 +6730,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="83" spans="1:8" hidden="1">
+    <row r="83" spans="1:8">
       <c r="A83" s="8" t="s">
         <v>387</v>
       </c>
@@ -6754,7 +6756,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="84" spans="1:8" hidden="1">
+    <row r="84" spans="1:8">
       <c r="A84" s="8" t="s">
         <v>387</v>
       </c>
@@ -6780,7 +6782,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="85" spans="1:8" hidden="1">
+    <row r="85" spans="1:8">
       <c r="A85" s="8" t="s">
         <v>387</v>
       </c>
@@ -6806,7 +6808,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="86" spans="1:8" hidden="1">
+    <row r="86" spans="1:8">
       <c r="A86" s="8" t="s">
         <v>387</v>
       </c>
@@ -6832,7 +6834,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="87" spans="1:8" hidden="1">
+    <row r="87" spans="1:8">
       <c r="A87" s="8" t="s">
         <v>388</v>
       </c>
@@ -6858,7 +6860,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="88" spans="1:8" hidden="1">
+    <row r="88" spans="1:8">
       <c r="A88" s="8" t="s">
         <v>388</v>
       </c>
@@ -6884,7 +6886,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="89" spans="1:8" hidden="1">
+    <row r="89" spans="1:8">
       <c r="A89" s="8" t="s">
         <v>388</v>
       </c>
@@ -6910,7 +6912,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="90" spans="1:8" hidden="1">
+    <row r="90" spans="1:8">
       <c r="A90" s="8" t="s">
         <v>388</v>
       </c>
@@ -6936,7 +6938,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="91" spans="1:8" hidden="1">
+    <row r="91" spans="1:8">
       <c r="A91" s="8" t="s">
         <v>388</v>
       </c>
@@ -6962,7 +6964,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="92" spans="1:8" hidden="1">
+    <row r="92" spans="1:8">
       <c r="A92" s="8" t="s">
         <v>388</v>
       </c>
@@ -6988,7 +6990,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="93" spans="1:8" hidden="1">
+    <row r="93" spans="1:8">
       <c r="A93" s="8" t="s">
         <v>388</v>
       </c>
@@ -7014,7 +7016,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="94" spans="1:8" hidden="1">
+    <row r="94" spans="1:8">
       <c r="A94" s="8" t="s">
         <v>388</v>
       </c>
@@ -7040,7 +7042,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="95" spans="1:8" hidden="1">
+    <row r="95" spans="1:8">
       <c r="A95" s="8" t="s">
         <v>388</v>
       </c>
@@ -7066,7 +7068,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="96" spans="1:8" hidden="1">
+    <row r="96" spans="1:8">
       <c r="A96" s="8" t="s">
         <v>388</v>
       </c>
@@ -7092,7 +7094,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="97" spans="1:8" hidden="1">
+    <row r="97" spans="1:8">
       <c r="A97" s="8" t="s">
         <v>388</v>
       </c>
@@ -7118,7 +7120,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="98" spans="1:8" hidden="1">
+    <row r="98" spans="1:8">
       <c r="A98" s="8" t="s">
         <v>388</v>
       </c>
@@ -7144,7 +7146,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="99" spans="1:8" hidden="1">
+    <row r="99" spans="1:8">
       <c r="A99" s="8" t="s">
         <v>388</v>
       </c>
@@ -7170,7 +7172,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="100" spans="1:8" hidden="1">
+    <row r="100" spans="1:8">
       <c r="A100" s="8" t="s">
         <v>388</v>
       </c>
@@ -7196,7 +7198,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="101" spans="1:8" hidden="1">
+    <row r="101" spans="1:8">
       <c r="A101" s="8" t="s">
         <v>388</v>
       </c>
@@ -7222,7 +7224,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="102" spans="1:8" hidden="1">
+    <row r="102" spans="1:8">
       <c r="A102" s="8" t="s">
         <v>389</v>
       </c>
@@ -7248,7 +7250,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="103" spans="1:8" hidden="1">
+    <row r="103" spans="1:8">
       <c r="A103" s="8" t="s">
         <v>389</v>
       </c>
@@ -7274,7 +7276,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="104" spans="1:8" hidden="1">
+    <row r="104" spans="1:8">
       <c r="A104" s="8" t="s">
         <v>389</v>
       </c>
@@ -7300,7 +7302,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="105" spans="1:8" hidden="1">
+    <row r="105" spans="1:8">
       <c r="A105" s="8" t="s">
         <v>389</v>
       </c>
@@ -7326,7 +7328,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="106" spans="1:8" hidden="1">
+    <row r="106" spans="1:8">
       <c r="A106" s="8" t="s">
         <v>389</v>
       </c>
@@ -7352,7 +7354,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="107" spans="1:8" hidden="1">
+    <row r="107" spans="1:8">
       <c r="A107" s="8" t="s">
         <v>389</v>
       </c>
@@ -7378,7 +7380,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="108" spans="1:8" hidden="1">
+    <row r="108" spans="1:8">
       <c r="A108" s="8" t="s">
         <v>389</v>
       </c>
@@ -7404,7 +7406,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="109" spans="1:8" hidden="1">
+    <row r="109" spans="1:8">
       <c r="A109" s="8" t="s">
         <v>389</v>
       </c>
@@ -7430,7 +7432,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="110" spans="1:8" hidden="1">
+    <row r="110" spans="1:8">
       <c r="A110" s="8" t="s">
         <v>389</v>
       </c>
@@ -7456,7 +7458,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="111" spans="1:8" hidden="1">
+    <row r="111" spans="1:8">
       <c r="A111" s="8" t="s">
         <v>389</v>
       </c>
@@ -7482,7 +7484,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="112" spans="1:8" hidden="1">
+    <row r="112" spans="1:8">
       <c r="A112" s="8" t="s">
         <v>389</v>
       </c>
@@ -7742,7 +7744,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="122" spans="1:8" hidden="1">
+    <row r="122" spans="1:8">
       <c r="A122" s="8" t="s">
         <v>391</v>
       </c>
@@ -7768,7 +7770,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="123" spans="1:8" hidden="1">
+    <row r="123" spans="1:8">
       <c r="A123" s="8" t="s">
         <v>391</v>
       </c>
@@ -7794,7 +7796,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="124" spans="1:8" hidden="1">
+    <row r="124" spans="1:8">
       <c r="A124" s="8" t="s">
         <v>391</v>
       </c>
@@ -7820,7 +7822,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="125" spans="1:8" hidden="1">
+    <row r="125" spans="1:8">
       <c r="A125" s="8" t="s">
         <v>391</v>
       </c>
@@ -7846,7 +7848,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="126" spans="1:8" hidden="1">
+    <row r="126" spans="1:8">
       <c r="A126" s="8" t="s">
         <v>391</v>
       </c>
@@ -7872,7 +7874,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="127" spans="1:8" hidden="1">
+    <row r="127" spans="1:8">
       <c r="A127" s="8" t="s">
         <v>391</v>
       </c>
@@ -7898,7 +7900,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="128" spans="1:8" hidden="1">
+    <row r="128" spans="1:8">
       <c r="A128" s="8" t="s">
         <v>391</v>
       </c>
@@ -7924,7 +7926,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="129" spans="1:8" hidden="1">
+    <row r="129" spans="1:8">
       <c r="A129" s="8" t="s">
         <v>391</v>
       </c>
@@ -7950,7 +7952,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="130" spans="1:8" hidden="1">
+    <row r="130" spans="1:8">
       <c r="A130" s="8" t="s">
         <v>391</v>
       </c>
@@ -7976,7 +7978,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="131" spans="1:8" hidden="1">
+    <row r="131" spans="1:8">
       <c r="A131" s="8" t="s">
         <v>391</v>
       </c>
@@ -8002,7 +8004,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="132" spans="1:8" hidden="1">
+    <row r="132" spans="1:8">
       <c r="A132" s="8" t="s">
         <v>391</v>
       </c>
@@ -8028,7 +8030,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="133" spans="1:8" hidden="1">
+    <row r="133" spans="1:8">
       <c r="A133" s="8" t="s">
         <v>391</v>
       </c>
@@ -8054,7 +8056,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="134" spans="1:8" hidden="1">
+    <row r="134" spans="1:8">
       <c r="A134" s="8" t="s">
         <v>391</v>
       </c>
@@ -8080,7 +8082,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="135" spans="1:8" hidden="1">
+    <row r="135" spans="1:8">
       <c r="A135" s="8" t="s">
         <v>391</v>
       </c>
@@ -8106,7 +8108,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="136" spans="1:8" hidden="1">
+    <row r="136" spans="1:8">
       <c r="A136" s="8" t="s">
         <v>391</v>
       </c>
@@ -8132,7 +8134,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="137" spans="1:8" hidden="1">
+    <row r="137" spans="1:8">
       <c r="A137" s="8" t="s">
         <v>391</v>
       </c>
@@ -8158,7 +8160,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="138" spans="1:8" hidden="1">
+    <row r="138" spans="1:8">
       <c r="A138" s="8" t="s">
         <v>391</v>
       </c>
@@ -8184,7 +8186,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="139" spans="1:8" hidden="1">
+    <row r="139" spans="1:8">
       <c r="A139" s="8" t="s">
         <v>391</v>
       </c>
@@ -8210,7 +8212,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="140" spans="1:8" hidden="1">
+    <row r="140" spans="1:8">
       <c r="A140" s="8" t="s">
         <v>391</v>
       </c>
@@ -8236,7 +8238,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="141" spans="1:8" hidden="1">
+    <row r="141" spans="1:8">
       <c r="A141" s="8" t="s">
         <v>391</v>
       </c>
@@ -8262,7 +8264,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="142" spans="1:8" hidden="1">
+    <row r="142" spans="1:8">
       <c r="A142" s="8" t="s">
         <v>391</v>
       </c>
@@ -8288,7 +8290,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="143" spans="1:8" hidden="1">
+    <row r="143" spans="1:8">
       <c r="A143" s="8" t="s">
         <v>391</v>
       </c>
@@ -8314,7 +8316,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="144" spans="1:8" hidden="1">
+    <row r="144" spans="1:8">
       <c r="A144" s="8" t="s">
         <v>391</v>
       </c>
@@ -8340,7 +8342,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="145" spans="1:8" hidden="1">
+    <row r="145" spans="1:8">
       <c r="A145" s="8" t="s">
         <v>391</v>
       </c>
@@ -8366,7 +8368,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="146" spans="1:8" hidden="1">
+    <row r="146" spans="1:8">
       <c r="A146" s="8" t="s">
         <v>391</v>
       </c>
@@ -8392,7 +8394,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="147" spans="1:8" hidden="1">
+    <row r="147" spans="1:8">
       <c r="A147" s="8" t="s">
         <v>391</v>
       </c>
@@ -8418,7 +8420,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="148" spans="1:8" hidden="1">
+    <row r="148" spans="1:8">
       <c r="A148" s="8" t="s">
         <v>391</v>
       </c>
@@ -8444,7 +8446,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="149" spans="1:8" hidden="1">
+    <row r="149" spans="1:8">
       <c r="A149" s="8" t="s">
         <v>391</v>
       </c>
@@ -8470,7 +8472,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="150" spans="1:8" hidden="1">
+    <row r="150" spans="1:8">
       <c r="A150" s="8" t="s">
         <v>391</v>
       </c>
@@ -8496,7 +8498,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="151" spans="1:8" hidden="1">
+    <row r="151" spans="1:8">
       <c r="A151" s="8" t="s">
         <v>391</v>
       </c>
@@ -8522,7 +8524,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="152" spans="1:8" hidden="1">
+    <row r="152" spans="1:8">
       <c r="A152" s="8" t="s">
         <v>391</v>
       </c>
@@ -8548,7 +8550,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="153" spans="1:8" hidden="1">
+    <row r="153" spans="1:8">
       <c r="A153" s="8" t="s">
         <v>391</v>
       </c>
@@ -8574,9 +8576,9 @@
         <v>934</v>
       </c>
     </row>
-    <row r="154" spans="1:8" hidden="1">
-      <c r="A154" s="8" t="s">
-        <v>391</v>
+    <row r="154" spans="1:8">
+      <c r="A154" t="s">
+        <v>1186</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>286</v>
@@ -8600,7 +8602,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="155" spans="1:8" hidden="1">
+    <row r="155" spans="1:8">
       <c r="A155" s="8" t="s">
         <v>391</v>
       </c>
@@ -8626,9 +8628,9 @@
         <v>936</v>
       </c>
     </row>
-    <row r="156" spans="1:8" hidden="1">
-      <c r="A156" s="8" t="s">
-        <v>391</v>
+    <row r="156" spans="1:8">
+      <c r="A156" t="s">
+        <v>1186</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>1139</v>
@@ -8652,9 +8654,9 @@
         <v>937</v>
       </c>
     </row>
-    <row r="157" spans="1:8" hidden="1">
-      <c r="A157" s="8" t="s">
-        <v>391</v>
+    <row r="157" spans="1:8">
+      <c r="A157" t="s">
+        <v>1186</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>1140</v>
@@ -8678,9 +8680,9 @@
         <v>939</v>
       </c>
     </row>
-    <row r="158" spans="1:8" hidden="1">
-      <c r="A158" s="8" t="s">
-        <v>391</v>
+    <row r="158" spans="1:8">
+      <c r="A158" t="s">
+        <v>1186</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>525</v>
@@ -8704,9 +8706,9 @@
         <v>942</v>
       </c>
     </row>
-    <row r="159" spans="1:8" hidden="1">
-      <c r="A159" s="8" t="s">
-        <v>391</v>
+    <row r="159" spans="1:8">
+      <c r="A159" t="s">
+        <v>1186</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>1141</v>
@@ -8730,9 +8732,9 @@
         <v>943</v>
       </c>
     </row>
-    <row r="160" spans="1:8" hidden="1">
-      <c r="A160" s="8" t="s">
-        <v>391</v>
+    <row r="160" spans="1:8">
+      <c r="A160" t="s">
+        <v>1186</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>1142</v>
@@ -8756,9 +8758,9 @@
         <v>945</v>
       </c>
     </row>
-    <row r="161" spans="1:8" hidden="1">
-      <c r="A161" s="8" t="s">
-        <v>391</v>
+    <row r="161" spans="1:8">
+      <c r="A161" t="s">
+        <v>1186</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>1143</v>
@@ -8782,9 +8784,9 @@
         <v>947</v>
       </c>
     </row>
-    <row r="162" spans="1:8" hidden="1">
-      <c r="A162" s="8" t="s">
-        <v>391</v>
+    <row r="162" spans="1:8">
+      <c r="A162" t="s">
+        <v>1186</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>1144</v>
@@ -8808,9 +8810,9 @@
         <v>948</v>
       </c>
     </row>
-    <row r="163" spans="1:8" hidden="1">
-      <c r="A163" s="8" t="s">
-        <v>391</v>
+    <row r="163" spans="1:8">
+      <c r="A163" t="s">
+        <v>1186</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>1145</v>
@@ -8834,9 +8836,9 @@
         <v>951</v>
       </c>
     </row>
-    <row r="164" spans="1:8" hidden="1">
-      <c r="A164" s="8" t="s">
-        <v>391</v>
+    <row r="164" spans="1:8">
+      <c r="A164" t="s">
+        <v>1186</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>543</v>
@@ -8860,7 +8862,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="165" spans="1:8" hidden="1">
+    <row r="165" spans="1:8">
       <c r="A165" s="8" t="s">
         <v>391</v>
       </c>
@@ -8886,7 +8888,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="166" spans="1:8" hidden="1">
+    <row r="166" spans="1:8">
       <c r="A166" s="8" t="s">
         <v>391</v>
       </c>
@@ -8912,7 +8914,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="167" spans="1:8" hidden="1">
+    <row r="167" spans="1:8">
       <c r="A167" s="8" t="s">
         <v>391</v>
       </c>
@@ -8938,7 +8940,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="168" spans="1:8" hidden="1">
+    <row r="168" spans="1:8">
       <c r="A168" s="8" t="s">
         <v>391</v>
       </c>
@@ -8964,7 +8966,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="169" spans="1:8" hidden="1">
+    <row r="169" spans="1:8">
       <c r="A169" s="8" t="s">
         <v>391</v>
       </c>
@@ -8990,7 +8992,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="170" spans="1:8" hidden="1">
+    <row r="170" spans="1:8">
       <c r="A170" s="8" t="s">
         <v>391</v>
       </c>
@@ -9016,7 +9018,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="171" spans="1:8" hidden="1">
+    <row r="171" spans="1:8">
       <c r="A171" s="8" t="s">
         <v>391</v>
       </c>
@@ -9042,7 +9044,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="172" spans="1:8" hidden="1">
+    <row r="172" spans="1:8">
       <c r="A172" s="8" t="s">
         <v>391</v>
       </c>
@@ -9068,7 +9070,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="173" spans="1:8" hidden="1">
+    <row r="173" spans="1:8">
       <c r="A173" s="8" t="s">
         <v>391</v>
       </c>
@@ -9094,7 +9096,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="174" spans="1:8" hidden="1">
+    <row r="174" spans="1:8">
       <c r="A174" s="8" t="s">
         <v>391</v>
       </c>
@@ -9120,7 +9122,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="175" spans="1:8" hidden="1">
+    <row r="175" spans="1:8">
       <c r="A175" s="8" t="s">
         <v>391</v>
       </c>
@@ -9146,7 +9148,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="176" spans="1:8" hidden="1">
+    <row r="176" spans="1:8">
       <c r="A176" s="8" t="s">
         <v>391</v>
       </c>
@@ -9172,7 +9174,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="177" spans="1:8" hidden="1">
+    <row r="177" spans="1:8">
       <c r="A177" s="8" t="s">
         <v>391</v>
       </c>
@@ -9198,7 +9200,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="178" spans="1:8" hidden="1">
+    <row r="178" spans="1:8">
       <c r="A178" s="8" t="s">
         <v>391</v>
       </c>
@@ -9224,7 +9226,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="179" spans="1:8" hidden="1">
+    <row r="179" spans="1:8">
       <c r="A179" s="8" t="s">
         <v>391</v>
       </c>
@@ -9250,7 +9252,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="180" spans="1:8" hidden="1">
+    <row r="180" spans="1:8">
       <c r="A180" s="8" t="s">
         <v>391</v>
       </c>
@@ -9276,7 +9278,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="181" spans="1:8" hidden="1">
+    <row r="181" spans="1:8">
       <c r="A181" s="8" t="s">
         <v>391</v>
       </c>
@@ -9302,7 +9304,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="182" spans="1:8" hidden="1">
+    <row r="182" spans="1:8">
       <c r="A182" s="8" t="s">
         <v>391</v>
       </c>
@@ -9328,7 +9330,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="183" spans="1:8" hidden="1">
+    <row r="183" spans="1:8">
       <c r="A183" s="8" t="s">
         <v>391</v>
       </c>
@@ -9354,7 +9356,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="184" spans="1:8" hidden="1">
+    <row r="184" spans="1:8">
       <c r="A184" s="8" t="s">
         <v>391</v>
       </c>
@@ -9380,7 +9382,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="185" spans="1:8" hidden="1">
+    <row r="185" spans="1:8">
       <c r="A185" s="8" t="s">
         <v>391</v>
       </c>
@@ -9406,7 +9408,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="186" spans="1:8" hidden="1">
+    <row r="186" spans="1:8">
       <c r="A186" s="8" t="s">
         <v>391</v>
       </c>
@@ -9432,7 +9434,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="187" spans="1:8" hidden="1">
+    <row r="187" spans="1:8">
       <c r="A187" s="8" t="s">
         <v>391</v>
       </c>
@@ -9458,7 +9460,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="188" spans="1:8" hidden="1">
+    <row r="188" spans="1:8">
       <c r="A188" s="8" t="s">
         <v>391</v>
       </c>
@@ -9484,7 +9486,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="189" spans="1:8" hidden="1">
+    <row r="189" spans="1:8">
       <c r="A189" s="8" t="s">
         <v>391</v>
       </c>
@@ -9510,7 +9512,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="190" spans="1:8" hidden="1">
+    <row r="190" spans="1:8">
       <c r="A190" s="8" t="s">
         <v>391</v>
       </c>
@@ -9536,7 +9538,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="191" spans="1:8" hidden="1">
+    <row r="191" spans="1:8">
       <c r="A191" s="8" t="s">
         <v>391</v>
       </c>
@@ -9562,7 +9564,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="192" spans="1:8" hidden="1">
+    <row r="192" spans="1:8">
       <c r="A192" s="8" t="s">
         <v>391</v>
       </c>
@@ -9588,7 +9590,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="193" spans="1:8" hidden="1">
+    <row r="193" spans="1:8">
       <c r="A193" s="8" t="s">
         <v>391</v>
       </c>
@@ -9614,7 +9616,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="194" spans="1:8" hidden="1">
+    <row r="194" spans="1:8">
       <c r="A194" s="8" t="s">
         <v>391</v>
       </c>
@@ -9640,7 +9642,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="195" spans="1:8" hidden="1">
+    <row r="195" spans="1:8">
       <c r="A195" s="8" t="s">
         <v>391</v>
       </c>
@@ -9666,7 +9668,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="196" spans="1:8" hidden="1">
+    <row r="196" spans="1:8">
       <c r="A196" s="8" t="s">
         <v>391</v>
       </c>
@@ -9692,7 +9694,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="197" spans="1:8" hidden="1">
+    <row r="197" spans="1:8">
       <c r="A197" s="8" t="s">
         <v>391</v>
       </c>
@@ -9718,7 +9720,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="198" spans="1:8" hidden="1">
+    <row r="198" spans="1:8">
       <c r="A198" s="8" t="s">
         <v>391</v>
       </c>
@@ -9744,7 +9746,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="199" spans="1:8" hidden="1">
+    <row r="199" spans="1:8">
       <c r="A199" s="8" t="s">
         <v>391</v>
       </c>
@@ -9770,7 +9772,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="200" spans="1:8" hidden="1">
+    <row r="200" spans="1:8">
       <c r="A200" s="8" t="s">
         <v>391</v>
       </c>
@@ -9796,7 +9798,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="201" spans="1:8" hidden="1">
+    <row r="201" spans="1:8">
       <c r="A201" s="8" t="s">
         <v>391</v>
       </c>
@@ -9822,7 +9824,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="202" spans="1:8" hidden="1">
+    <row r="202" spans="1:8">
       <c r="A202" s="8" t="s">
         <v>391</v>
       </c>
@@ -9848,7 +9850,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="203" spans="1:8" hidden="1">
+    <row r="203" spans="1:8">
       <c r="A203" s="8" t="s">
         <v>391</v>
       </c>
@@ -9874,7 +9876,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="204" spans="1:8" hidden="1">
+    <row r="204" spans="1:8">
       <c r="A204" s="8" t="s">
         <v>391</v>
       </c>
@@ -9900,7 +9902,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="205" spans="1:8" hidden="1">
+    <row r="205" spans="1:8">
       <c r="A205" s="8" t="s">
         <v>391</v>
       </c>
@@ -9926,7 +9928,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="206" spans="1:8" hidden="1">
+    <row r="206" spans="1:8">
       <c r="A206" s="8" t="s">
         <v>391</v>
       </c>
@@ -9952,7 +9954,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="207" spans="1:8" hidden="1">
+    <row r="207" spans="1:8">
       <c r="A207" s="8" t="s">
         <v>391</v>
       </c>
@@ -9978,7 +9980,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="208" spans="1:8" hidden="1">
+    <row r="208" spans="1:8">
       <c r="A208" s="8" t="s">
         <v>391</v>
       </c>
@@ -10004,7 +10006,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="209" spans="1:8" hidden="1">
+    <row r="209" spans="1:8">
       <c r="A209" s="8" t="s">
         <v>391</v>
       </c>
@@ -10030,7 +10032,7 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="210" spans="1:8" hidden="1">
+    <row r="210" spans="1:8">
       <c r="A210" s="8" t="s">
         <v>391</v>
       </c>
@@ -10056,7 +10058,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="211" spans="1:8" hidden="1">
+    <row r="211" spans="1:8">
       <c r="A211" s="8" t="s">
         <v>391</v>
       </c>
@@ -10082,7 +10084,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="212" spans="1:8" hidden="1">
+    <row r="212" spans="1:8">
       <c r="A212" s="8" t="s">
         <v>391</v>
       </c>
@@ -10108,7 +10110,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="213" spans="1:8" hidden="1">
+    <row r="213" spans="1:8">
       <c r="A213" s="8" t="s">
         <v>391</v>
       </c>
@@ -10134,7 +10136,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="214" spans="1:8" hidden="1">
+    <row r="214" spans="1:8">
       <c r="A214" s="8" t="s">
         <v>391</v>
       </c>
@@ -10160,7 +10162,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="215" spans="1:8" hidden="1">
+    <row r="215" spans="1:8">
       <c r="A215" s="8" t="s">
         <v>391</v>
       </c>
@@ -10186,7 +10188,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="216" spans="1:8" hidden="1">
+    <row r="216" spans="1:8">
       <c r="A216" s="8" t="s">
         <v>391</v>
       </c>
@@ -10212,7 +10214,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="217" spans="1:8" hidden="1">
+    <row r="217" spans="1:8">
       <c r="A217" s="8" t="s">
         <v>391</v>
       </c>
@@ -10238,7 +10240,7 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="218" spans="1:8" hidden="1">
+    <row r="218" spans="1:8">
       <c r="A218" s="8" t="s">
         <v>391</v>
       </c>
@@ -10264,7 +10266,7 @@
         <v>1123</v>
       </c>
     </row>
-    <row r="219" spans="1:8" hidden="1">
+    <row r="219" spans="1:8">
       <c r="A219" s="8" t="s">
         <v>391</v>
       </c>
@@ -10291,18 +10293,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H219" xr:uid="{0FC232BA-84F4-BE49-B367-4C71587DA4B6}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Medication Management"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <conditionalFormatting sqref="D1">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D1">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="C16" r:id="rId1" display="https://www.mayoclinic.org/healthy-lifestyle/recipes/chicken-fajitas/rcp-20049943." xr:uid="{BF040B87-8534-9445-90AC-FE2659D40410}"/>

</xml_diff>

<commit_message>
updating code for Spanish bugs
</commit_message>
<xml_diff>
--- a/responses.xlsx
+++ b/responses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshvasilvasstar/Documents/clinicchat/dh-c4h-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{064BEC13-2A17-CC41-B368-559FF77FEAF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF623E3F-5BB2-CB4A-87D3-ECE15F291936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5900" yWindow="9820" windowWidth="27640" windowHeight="16940" xr2:uid="{E7C9F955-17B0-F040-8EA4-EA009C6A7680}"/>
+    <workbookView xWindow="2700" yWindow="3920" windowWidth="27640" windowHeight="16940" xr2:uid="{E7C9F955-17B0-F040-8EA4-EA009C6A7680}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4585,10 +4585,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC232BA-84F4-BE49-B367-4C71587DA4B6}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H219"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A154" sqref="A154:A164"/>
+      <selection activeCell="B164" sqref="B164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4624,7 +4625,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" hidden="1">
       <c r="A2" s="8" t="s">
         <v>384</v>
       </c>
@@ -4650,7 +4651,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" hidden="1">
       <c r="A3" s="8" t="s">
         <v>384</v>
       </c>
@@ -4676,7 +4677,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" hidden="1">
       <c r="A4" s="8" t="s">
         <v>391</v>
       </c>
@@ -4702,7 +4703,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" hidden="1">
       <c r="A5" s="8" t="s">
         <v>391</v>
       </c>
@@ -4728,7 +4729,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" hidden="1">
       <c r="A6" s="8" t="s">
         <v>391</v>
       </c>
@@ -4754,7 +4755,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" hidden="1">
       <c r="A7" s="8" t="s">
         <v>391</v>
       </c>
@@ -4780,7 +4781,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" hidden="1">
       <c r="A8" s="8" t="s">
         <v>391</v>
       </c>
@@ -4806,7 +4807,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" hidden="1">
       <c r="A9" s="8" t="s">
         <v>391</v>
       </c>
@@ -4832,7 +4833,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" hidden="1">
       <c r="A10" s="8" t="s">
         <v>391</v>
       </c>
@@ -4858,7 +4859,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" hidden="1">
       <c r="A11" s="8" t="s">
         <v>383</v>
       </c>
@@ -4884,7 +4885,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" hidden="1">
       <c r="A12" s="8" t="s">
         <v>383</v>
       </c>
@@ -4910,7 +4911,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" hidden="1">
       <c r="A13" s="8" t="s">
         <v>383</v>
       </c>
@@ -4936,7 +4937,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" hidden="1">
       <c r="A14" s="8" t="s">
         <v>383</v>
       </c>
@@ -4962,7 +4963,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" hidden="1">
       <c r="A15" s="8" t="s">
         <v>383</v>
       </c>
@@ -4988,7 +4989,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" hidden="1">
       <c r="A16" s="8" t="s">
         <v>383</v>
       </c>
@@ -5014,7 +5015,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" hidden="1">
       <c r="A17" s="8" t="s">
         <v>383</v>
       </c>
@@ -5040,7 +5041,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" hidden="1">
       <c r="A18" s="8" t="s">
         <v>383</v>
       </c>
@@ -5066,7 +5067,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" hidden="1">
       <c r="A19" s="8" t="s">
         <v>383</v>
       </c>
@@ -5092,7 +5093,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" hidden="1">
       <c r="A20" s="8" t="s">
         <v>383</v>
       </c>
@@ -5118,7 +5119,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" hidden="1">
       <c r="A21" s="8" t="s">
         <v>383</v>
       </c>
@@ -5144,7 +5145,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" hidden="1">
       <c r="A22" s="8" t="s">
         <v>383</v>
       </c>
@@ -5170,7 +5171,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" hidden="1">
       <c r="A23" s="8" t="s">
         <v>383</v>
       </c>
@@ -5196,7 +5197,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" hidden="1">
       <c r="A24" s="8" t="s">
         <v>383</v>
       </c>
@@ -5222,7 +5223,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" hidden="1">
       <c r="A25" s="8" t="s">
         <v>383</v>
       </c>
@@ -5248,7 +5249,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" hidden="1">
       <c r="A26" s="8" t="s">
         <v>383</v>
       </c>
@@ -5274,7 +5275,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" hidden="1">
       <c r="A27" s="8" t="s">
         <v>383</v>
       </c>
@@ -5300,7 +5301,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" hidden="1">
       <c r="A28" s="8" t="s">
         <v>383</v>
       </c>
@@ -5326,7 +5327,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" hidden="1">
       <c r="A29" s="8" t="s">
         <v>383</v>
       </c>
@@ -5352,7 +5353,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" hidden="1">
       <c r="A30" s="8" t="s">
         <v>384</v>
       </c>
@@ -5378,7 +5379,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" hidden="1">
       <c r="A31" s="8" t="s">
         <v>384</v>
       </c>
@@ -5404,7 +5405,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" hidden="1">
       <c r="A32" s="8" t="s">
         <v>384</v>
       </c>
@@ -5430,7 +5431,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" hidden="1">
       <c r="A33" s="8" t="s">
         <v>384</v>
       </c>
@@ -5456,7 +5457,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" hidden="1">
       <c r="A34" s="8" t="s">
         <v>384</v>
       </c>
@@ -5482,7 +5483,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" hidden="1">
       <c r="A35" s="8" t="s">
         <v>384</v>
       </c>
@@ -5508,7 +5509,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" hidden="1">
       <c r="A36" s="8" t="s">
         <v>384</v>
       </c>
@@ -5534,7 +5535,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" hidden="1">
       <c r="A37" s="8" t="s">
         <v>384</v>
       </c>
@@ -5560,7 +5561,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" hidden="1">
       <c r="A38" s="8" t="s">
         <v>384</v>
       </c>
@@ -5586,7 +5587,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" hidden="1">
       <c r="A39" s="8" t="s">
         <v>384</v>
       </c>
@@ -5612,7 +5613,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" hidden="1">
       <c r="A40" s="8" t="s">
         <v>384</v>
       </c>
@@ -5638,7 +5639,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" hidden="1">
       <c r="A41" s="8" t="s">
         <v>384</v>
       </c>
@@ -5664,7 +5665,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" hidden="1">
       <c r="A42" s="8" t="s">
         <v>384</v>
       </c>
@@ -5690,7 +5691,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" hidden="1">
       <c r="A43" s="8" t="s">
         <v>384</v>
       </c>
@@ -5716,7 +5717,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" hidden="1">
       <c r="A44" s="8" t="s">
         <v>384</v>
       </c>
@@ -5742,7 +5743,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" hidden="1">
       <c r="A45" s="8" t="s">
         <v>384</v>
       </c>
@@ -5768,7 +5769,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" hidden="1">
       <c r="A46" s="8" t="s">
         <v>384</v>
       </c>
@@ -5794,7 +5795,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" hidden="1">
       <c r="A47" s="8" t="s">
         <v>384</v>
       </c>
@@ -5820,7 +5821,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" hidden="1">
       <c r="A48" s="8" t="s">
         <v>384</v>
       </c>
@@ -5846,7 +5847,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" hidden="1">
       <c r="A49" s="8" t="s">
         <v>384</v>
       </c>
@@ -5872,7 +5873,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" hidden="1">
       <c r="A50" s="8" t="s">
         <v>384</v>
       </c>
@@ -5898,7 +5899,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" hidden="1">
       <c r="A51" s="8" t="s">
         <v>384</v>
       </c>
@@ -5924,7 +5925,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" hidden="1">
       <c r="A52" s="8" t="s">
         <v>384</v>
       </c>
@@ -5950,7 +5951,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" hidden="1">
       <c r="A53" s="8" t="s">
         <v>384</v>
       </c>
@@ -5976,7 +5977,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" hidden="1">
       <c r="A54" s="8" t="s">
         <v>384</v>
       </c>
@@ -6002,7 +6003,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" hidden="1">
       <c r="A55" s="8" t="s">
         <v>384</v>
       </c>
@@ -6028,7 +6029,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" hidden="1">
       <c r="A56" s="8" t="s">
         <v>384</v>
       </c>
@@ -6054,7 +6055,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" hidden="1">
       <c r="A57" s="8" t="s">
         <v>384</v>
       </c>
@@ -6080,7 +6081,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" hidden="1">
       <c r="A58" s="8" t="s">
         <v>384</v>
       </c>
@@ -6106,7 +6107,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" hidden="1">
       <c r="A59" s="8" t="s">
         <v>385</v>
       </c>
@@ -6132,7 +6133,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" hidden="1">
       <c r="A60" s="8" t="s">
         <v>385</v>
       </c>
@@ -6158,7 +6159,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" hidden="1">
       <c r="A61" s="8" t="s">
         <v>385</v>
       </c>
@@ -6184,7 +6185,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" hidden="1">
       <c r="A62" s="8" t="s">
         <v>385</v>
       </c>
@@ -6210,7 +6211,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" hidden="1">
       <c r="A63" s="8" t="s">
         <v>385</v>
       </c>
@@ -6236,7 +6237,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" hidden="1">
       <c r="A64" s="8" t="s">
         <v>385</v>
       </c>
@@ -6262,7 +6263,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" hidden="1">
       <c r="A65" s="8" t="s">
         <v>385</v>
       </c>
@@ -6288,7 +6289,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" hidden="1">
       <c r="A66" s="8" t="s">
         <v>385</v>
       </c>
@@ -6314,7 +6315,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" hidden="1">
       <c r="A67" s="8" t="s">
         <v>386</v>
       </c>
@@ -6340,7 +6341,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" hidden="1">
       <c r="A68" s="8" t="s">
         <v>386</v>
       </c>
@@ -6366,7 +6367,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" hidden="1">
       <c r="A69" s="8" t="s">
         <v>386</v>
       </c>
@@ -6392,7 +6393,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" hidden="1">
       <c r="A70" s="8" t="s">
         <v>386</v>
       </c>
@@ -6418,7 +6419,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" hidden="1">
       <c r="A71" s="8" t="s">
         <v>386</v>
       </c>
@@ -6444,7 +6445,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" hidden="1">
       <c r="A72" s="8" t="s">
         <v>386</v>
       </c>
@@ -6470,7 +6471,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" hidden="1">
       <c r="A73" s="8" t="s">
         <v>386</v>
       </c>
@@ -6496,7 +6497,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" hidden="1">
       <c r="A74" s="8" t="s">
         <v>386</v>
       </c>
@@ -6522,7 +6523,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" hidden="1">
       <c r="A75" s="8" t="s">
         <v>386</v>
       </c>
@@ -6548,7 +6549,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" hidden="1">
       <c r="A76" s="8" t="s">
         <v>386</v>
       </c>
@@ -6574,7 +6575,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" hidden="1">
       <c r="A77" s="8" t="s">
         <v>386</v>
       </c>
@@ -6600,7 +6601,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" hidden="1">
       <c r="A78" s="8" t="s">
         <v>386</v>
       </c>
@@ -6626,7 +6627,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" hidden="1">
       <c r="A79" s="8" t="s">
         <v>387</v>
       </c>
@@ -6652,7 +6653,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" hidden="1">
       <c r="A80" s="8" t="s">
         <v>387</v>
       </c>
@@ -6678,7 +6679,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" hidden="1">
       <c r="A81" s="8" t="s">
         <v>387</v>
       </c>
@@ -6704,7 +6705,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" hidden="1">
       <c r="A82" s="8" t="s">
         <v>387</v>
       </c>
@@ -6730,7 +6731,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" hidden="1">
       <c r="A83" s="8" t="s">
         <v>387</v>
       </c>
@@ -6756,7 +6757,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" hidden="1">
       <c r="A84" s="8" t="s">
         <v>387</v>
       </c>
@@ -6782,7 +6783,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" hidden="1">
       <c r="A85" s="8" t="s">
         <v>387</v>
       </c>
@@ -6808,7 +6809,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" hidden="1">
       <c r="A86" s="8" t="s">
         <v>387</v>
       </c>
@@ -6834,7 +6835,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" hidden="1">
       <c r="A87" s="8" t="s">
         <v>388</v>
       </c>
@@ -6860,7 +6861,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" hidden="1">
       <c r="A88" s="8" t="s">
         <v>388</v>
       </c>
@@ -6886,7 +6887,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" hidden="1">
       <c r="A89" s="8" t="s">
         <v>388</v>
       </c>
@@ -6912,7 +6913,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" hidden="1">
       <c r="A90" s="8" t="s">
         <v>388</v>
       </c>
@@ -6938,7 +6939,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" hidden="1">
       <c r="A91" s="8" t="s">
         <v>388</v>
       </c>
@@ -6964,7 +6965,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" hidden="1">
       <c r="A92" s="8" t="s">
         <v>388</v>
       </c>
@@ -6990,7 +6991,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" hidden="1">
       <c r="A93" s="8" t="s">
         <v>388</v>
       </c>
@@ -7016,7 +7017,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" hidden="1">
       <c r="A94" s="8" t="s">
         <v>388</v>
       </c>
@@ -7042,7 +7043,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" hidden="1">
       <c r="A95" s="8" t="s">
         <v>388</v>
       </c>
@@ -7068,7 +7069,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" hidden="1">
       <c r="A96" s="8" t="s">
         <v>388</v>
       </c>
@@ -7094,7 +7095,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" hidden="1">
       <c r="A97" s="8" t="s">
         <v>388</v>
       </c>
@@ -7120,7 +7121,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" hidden="1">
       <c r="A98" s="8" t="s">
         <v>388</v>
       </c>
@@ -7146,7 +7147,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" hidden="1">
       <c r="A99" s="8" t="s">
         <v>388</v>
       </c>
@@ -7172,7 +7173,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" hidden="1">
       <c r="A100" s="8" t="s">
         <v>388</v>
       </c>
@@ -7198,7 +7199,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" hidden="1">
       <c r="A101" s="8" t="s">
         <v>388</v>
       </c>
@@ -7224,7 +7225,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" hidden="1">
       <c r="A102" s="8" t="s">
         <v>389</v>
       </c>
@@ -7250,7 +7251,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" hidden="1">
       <c r="A103" s="8" t="s">
         <v>389</v>
       </c>
@@ -7276,7 +7277,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" hidden="1">
       <c r="A104" s="8" t="s">
         <v>389</v>
       </c>
@@ -7302,7 +7303,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" hidden="1">
       <c r="A105" s="8" t="s">
         <v>389</v>
       </c>
@@ -7328,7 +7329,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" hidden="1">
       <c r="A106" s="8" t="s">
         <v>389</v>
       </c>
@@ -7354,7 +7355,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:8" hidden="1">
       <c r="A107" s="8" t="s">
         <v>389</v>
       </c>
@@ -7380,7 +7381,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:8" hidden="1">
       <c r="A108" s="8" t="s">
         <v>389</v>
       </c>
@@ -7406,7 +7407,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" hidden="1">
       <c r="A109" s="8" t="s">
         <v>389</v>
       </c>
@@ -7432,7 +7433,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="110" spans="1:8">
+    <row r="110" spans="1:8" hidden="1">
       <c r="A110" s="8" t="s">
         <v>389</v>
       </c>
@@ -7458,7 +7459,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="111" spans="1:8">
+    <row r="111" spans="1:8" hidden="1">
       <c r="A111" s="8" t="s">
         <v>389</v>
       </c>
@@ -7484,7 +7485,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="112" spans="1:8">
+    <row r="112" spans="1:8" hidden="1">
       <c r="A112" s="8" t="s">
         <v>389</v>
       </c>
@@ -7510,7 +7511,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:8" hidden="1">
       <c r="A113" s="8" t="s">
         <v>390</v>
       </c>
@@ -7536,7 +7537,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:8" hidden="1">
       <c r="A114" s="8" t="s">
         <v>390</v>
       </c>
@@ -7562,7 +7563,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:8" hidden="1">
       <c r="A115" s="8" t="s">
         <v>390</v>
       </c>
@@ -7588,7 +7589,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:8" hidden="1">
       <c r="A116" s="8" t="s">
         <v>390</v>
       </c>
@@ -7614,7 +7615,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:8" hidden="1">
       <c r="A117" s="8" t="s">
         <v>390</v>
       </c>
@@ -7640,7 +7641,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:8" hidden="1">
       <c r="A118" s="8" t="s">
         <v>390</v>
       </c>
@@ -7666,7 +7667,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:8" hidden="1">
       <c r="A119" s="8" t="s">
         <v>390</v>
       </c>
@@ -7692,7 +7693,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:8" hidden="1">
       <c r="A120" s="8" t="s">
         <v>390</v>
       </c>
@@ -7718,7 +7719,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" spans="1:8" hidden="1">
       <c r="A121" s="8" t="s">
         <v>390</v>
       </c>
@@ -7744,7 +7745,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:8" hidden="1">
       <c r="A122" s="8" t="s">
         <v>391</v>
       </c>
@@ -7770,7 +7771,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:8" hidden="1">
       <c r="A123" s="8" t="s">
         <v>391</v>
       </c>
@@ -7796,7 +7797,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="124" spans="1:8">
+    <row r="124" spans="1:8" hidden="1">
       <c r="A124" s="8" t="s">
         <v>391</v>
       </c>
@@ -7822,7 +7823,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="125" spans="1:8">
+    <row r="125" spans="1:8" hidden="1">
       <c r="A125" s="8" t="s">
         <v>391</v>
       </c>
@@ -7848,7 +7849,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="126" spans="1:8">
+    <row r="126" spans="1:8" hidden="1">
       <c r="A126" s="8" t="s">
         <v>391</v>
       </c>
@@ -7874,7 +7875,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="127" spans="1:8">
+    <row r="127" spans="1:8" hidden="1">
       <c r="A127" s="8" t="s">
         <v>391</v>
       </c>
@@ -7900,7 +7901,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="128" spans="1:8">
+    <row r="128" spans="1:8" hidden="1">
       <c r="A128" s="8" t="s">
         <v>391</v>
       </c>
@@ -7926,7 +7927,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="129" spans="1:8">
+    <row r="129" spans="1:8" hidden="1">
       <c r="A129" s="8" t="s">
         <v>391</v>
       </c>
@@ -7952,7 +7953,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="130" spans="1:8">
+    <row r="130" spans="1:8" hidden="1">
       <c r="A130" s="8" t="s">
         <v>391</v>
       </c>
@@ -7978,7 +7979,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="131" spans="1:8">
+    <row r="131" spans="1:8" hidden="1">
       <c r="A131" s="8" t="s">
         <v>391</v>
       </c>
@@ -8004,7 +8005,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="132" spans="1:8">
+    <row r="132" spans="1:8" hidden="1">
       <c r="A132" s="8" t="s">
         <v>391</v>
       </c>
@@ -8030,7 +8031,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="133" spans="1:8">
+    <row r="133" spans="1:8" hidden="1">
       <c r="A133" s="8" t="s">
         <v>391</v>
       </c>
@@ -8056,7 +8057,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="134" spans="1:8">
+    <row r="134" spans="1:8" hidden="1">
       <c r="A134" s="8" t="s">
         <v>391</v>
       </c>
@@ -8082,7 +8083,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="135" spans="1:8">
+    <row r="135" spans="1:8" hidden="1">
       <c r="A135" s="8" t="s">
         <v>391</v>
       </c>
@@ -8108,7 +8109,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="136" spans="1:8">
+    <row r="136" spans="1:8" hidden="1">
       <c r="A136" s="8" t="s">
         <v>391</v>
       </c>
@@ -8134,7 +8135,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="137" spans="1:8">
+    <row r="137" spans="1:8" hidden="1">
       <c r="A137" s="8" t="s">
         <v>391</v>
       </c>
@@ -8160,7 +8161,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="138" spans="1:8">
+    <row r="138" spans="1:8" hidden="1">
       <c r="A138" s="8" t="s">
         <v>391</v>
       </c>
@@ -8186,7 +8187,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="139" spans="1:8">
+    <row r="139" spans="1:8" hidden="1">
       <c r="A139" s="8" t="s">
         <v>391</v>
       </c>
@@ -8212,7 +8213,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="140" spans="1:8">
+    <row r="140" spans="1:8" hidden="1">
       <c r="A140" s="8" t="s">
         <v>391</v>
       </c>
@@ -8238,7 +8239,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="141" spans="1:8">
+    <row r="141" spans="1:8" hidden="1">
       <c r="A141" s="8" t="s">
         <v>391</v>
       </c>
@@ -8264,7 +8265,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="142" spans="1:8">
+    <row r="142" spans="1:8" hidden="1">
       <c r="A142" s="8" t="s">
         <v>391</v>
       </c>
@@ -8290,7 +8291,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="143" spans="1:8">
+    <row r="143" spans="1:8" hidden="1">
       <c r="A143" s="8" t="s">
         <v>391</v>
       </c>
@@ -8316,7 +8317,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="144" spans="1:8">
+    <row r="144" spans="1:8" hidden="1">
       <c r="A144" s="8" t="s">
         <v>391</v>
       </c>
@@ -8342,7 +8343,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="145" spans="1:8">
+    <row r="145" spans="1:8" hidden="1">
       <c r="A145" s="8" t="s">
         <v>391</v>
       </c>
@@ -8368,7 +8369,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="146" spans="1:8">
+    <row r="146" spans="1:8" hidden="1">
       <c r="A146" s="8" t="s">
         <v>391</v>
       </c>
@@ -8394,7 +8395,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="147" spans="1:8">
+    <row r="147" spans="1:8" hidden="1">
       <c r="A147" s="8" t="s">
         <v>391</v>
       </c>
@@ -8420,7 +8421,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="148" spans="1:8">
+    <row r="148" spans="1:8" hidden="1">
       <c r="A148" s="8" t="s">
         <v>391</v>
       </c>
@@ -8446,7 +8447,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="149" spans="1:8">
+    <row r="149" spans="1:8" hidden="1">
       <c r="A149" s="8" t="s">
         <v>391</v>
       </c>
@@ -8472,7 +8473,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="150" spans="1:8">
+    <row r="150" spans="1:8" hidden="1">
       <c r="A150" s="8" t="s">
         <v>391</v>
       </c>
@@ -8498,7 +8499,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="151" spans="1:8">
+    <row r="151" spans="1:8" hidden="1">
       <c r="A151" s="8" t="s">
         <v>391</v>
       </c>
@@ -8524,7 +8525,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="152" spans="1:8">
+    <row r="152" spans="1:8" hidden="1">
       <c r="A152" s="8" t="s">
         <v>391</v>
       </c>
@@ -8550,7 +8551,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="153" spans="1:8">
+    <row r="153" spans="1:8" hidden="1">
       <c r="A153" s="8" t="s">
         <v>391</v>
       </c>
@@ -8602,7 +8603,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="155" spans="1:8">
+    <row r="155" spans="1:8" hidden="1">
       <c r="A155" s="8" t="s">
         <v>391</v>
       </c>
@@ -8862,7 +8863,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="165" spans="1:8">
+    <row r="165" spans="1:8" hidden="1">
       <c r="A165" s="8" t="s">
         <v>391</v>
       </c>
@@ -8888,7 +8889,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="166" spans="1:8">
+    <row r="166" spans="1:8" hidden="1">
       <c r="A166" s="8" t="s">
         <v>391</v>
       </c>
@@ -8914,7 +8915,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="167" spans="1:8">
+    <row r="167" spans="1:8" hidden="1">
       <c r="A167" s="8" t="s">
         <v>391</v>
       </c>
@@ -8940,7 +8941,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="168" spans="1:8">
+    <row r="168" spans="1:8" hidden="1">
       <c r="A168" s="8" t="s">
         <v>391</v>
       </c>
@@ -8966,7 +8967,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="169" spans="1:8">
+    <row r="169" spans="1:8" hidden="1">
       <c r="A169" s="8" t="s">
         <v>391</v>
       </c>
@@ -8992,7 +8993,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="170" spans="1:8">
+    <row r="170" spans="1:8" hidden="1">
       <c r="A170" s="8" t="s">
         <v>391</v>
       </c>
@@ -9018,7 +9019,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="171" spans="1:8">
+    <row r="171" spans="1:8" hidden="1">
       <c r="A171" s="8" t="s">
         <v>391</v>
       </c>
@@ -9044,7 +9045,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="172" spans="1:8">
+    <row r="172" spans="1:8" hidden="1">
       <c r="A172" s="8" t="s">
         <v>391</v>
       </c>
@@ -9070,7 +9071,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="173" spans="1:8">
+    <row r="173" spans="1:8" hidden="1">
       <c r="A173" s="8" t="s">
         <v>391</v>
       </c>
@@ -9096,7 +9097,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="174" spans="1:8">
+    <row r="174" spans="1:8" hidden="1">
       <c r="A174" s="8" t="s">
         <v>391</v>
       </c>
@@ -9122,7 +9123,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="175" spans="1:8">
+    <row r="175" spans="1:8" hidden="1">
       <c r="A175" s="8" t="s">
         <v>391</v>
       </c>
@@ -9148,7 +9149,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="176" spans="1:8">
+    <row r="176" spans="1:8" hidden="1">
       <c r="A176" s="8" t="s">
         <v>391</v>
       </c>
@@ -9174,7 +9175,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="177" spans="1:8">
+    <row r="177" spans="1:8" hidden="1">
       <c r="A177" s="8" t="s">
         <v>391</v>
       </c>
@@ -9200,7 +9201,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="178" spans="1:8">
+    <row r="178" spans="1:8" hidden="1">
       <c r="A178" s="8" t="s">
         <v>391</v>
       </c>
@@ -9226,7 +9227,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="179" spans="1:8">
+    <row r="179" spans="1:8" hidden="1">
       <c r="A179" s="8" t="s">
         <v>391</v>
       </c>
@@ -9252,7 +9253,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="180" spans="1:8">
+    <row r="180" spans="1:8" hidden="1">
       <c r="A180" s="8" t="s">
         <v>391</v>
       </c>
@@ -9278,7 +9279,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="181" spans="1:8">
+    <row r="181" spans="1:8" hidden="1">
       <c r="A181" s="8" t="s">
         <v>391</v>
       </c>
@@ -9304,7 +9305,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="182" spans="1:8">
+    <row r="182" spans="1:8" hidden="1">
       <c r="A182" s="8" t="s">
         <v>391</v>
       </c>
@@ -9330,7 +9331,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="183" spans="1:8">
+    <row r="183" spans="1:8" hidden="1">
       <c r="A183" s="8" t="s">
         <v>391</v>
       </c>
@@ -9356,7 +9357,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="184" spans="1:8">
+    <row r="184" spans="1:8" hidden="1">
       <c r="A184" s="8" t="s">
         <v>391</v>
       </c>
@@ -9382,7 +9383,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="185" spans="1:8">
+    <row r="185" spans="1:8" hidden="1">
       <c r="A185" s="8" t="s">
         <v>391</v>
       </c>
@@ -9408,7 +9409,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="186" spans="1:8">
+    <row r="186" spans="1:8" hidden="1">
       <c r="A186" s="8" t="s">
         <v>391</v>
       </c>
@@ -9434,7 +9435,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="187" spans="1:8">
+    <row r="187" spans="1:8" hidden="1">
       <c r="A187" s="8" t="s">
         <v>391</v>
       </c>
@@ -9460,7 +9461,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="188" spans="1:8">
+    <row r="188" spans="1:8" hidden="1">
       <c r="A188" s="8" t="s">
         <v>391</v>
       </c>
@@ -9486,7 +9487,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="189" spans="1:8">
+    <row r="189" spans="1:8" hidden="1">
       <c r="A189" s="8" t="s">
         <v>391</v>
       </c>
@@ -9512,7 +9513,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="190" spans="1:8">
+    <row r="190" spans="1:8" hidden="1">
       <c r="A190" s="8" t="s">
         <v>391</v>
       </c>
@@ -9538,7 +9539,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="191" spans="1:8">
+    <row r="191" spans="1:8" hidden="1">
       <c r="A191" s="8" t="s">
         <v>391</v>
       </c>
@@ -9564,7 +9565,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="192" spans="1:8">
+    <row r="192" spans="1:8" hidden="1">
       <c r="A192" s="8" t="s">
         <v>391</v>
       </c>
@@ -9590,7 +9591,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="193" spans="1:8">
+    <row r="193" spans="1:8" hidden="1">
       <c r="A193" s="8" t="s">
         <v>391</v>
       </c>
@@ -9616,7 +9617,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="194" spans="1:8">
+    <row r="194" spans="1:8" hidden="1">
       <c r="A194" s="8" t="s">
         <v>391</v>
       </c>
@@ -9642,7 +9643,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="195" spans="1:8">
+    <row r="195" spans="1:8" hidden="1">
       <c r="A195" s="8" t="s">
         <v>391</v>
       </c>
@@ -9668,7 +9669,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="196" spans="1:8">
+    <row r="196" spans="1:8" hidden="1">
       <c r="A196" s="8" t="s">
         <v>391</v>
       </c>
@@ -9694,7 +9695,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="197" spans="1:8">
+    <row r="197" spans="1:8" hidden="1">
       <c r="A197" s="8" t="s">
         <v>391</v>
       </c>
@@ -9720,7 +9721,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="198" spans="1:8">
+    <row r="198" spans="1:8" hidden="1">
       <c r="A198" s="8" t="s">
         <v>391</v>
       </c>
@@ -9746,7 +9747,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="199" spans="1:8">
+    <row r="199" spans="1:8" hidden="1">
       <c r="A199" s="8" t="s">
         <v>391</v>
       </c>
@@ -9772,7 +9773,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="200" spans="1:8">
+    <row r="200" spans="1:8" hidden="1">
       <c r="A200" s="8" t="s">
         <v>391</v>
       </c>
@@ -9798,7 +9799,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="201" spans="1:8">
+    <row r="201" spans="1:8" hidden="1">
       <c r="A201" s="8" t="s">
         <v>391</v>
       </c>
@@ -9824,7 +9825,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="202" spans="1:8">
+    <row r="202" spans="1:8" hidden="1">
       <c r="A202" s="8" t="s">
         <v>391</v>
       </c>
@@ -9850,7 +9851,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="203" spans="1:8">
+    <row r="203" spans="1:8" hidden="1">
       <c r="A203" s="8" t="s">
         <v>391</v>
       </c>
@@ -9876,7 +9877,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="204" spans="1:8">
+    <row r="204" spans="1:8" hidden="1">
       <c r="A204" s="8" t="s">
         <v>391</v>
       </c>
@@ -9902,7 +9903,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="205" spans="1:8">
+    <row r="205" spans="1:8" hidden="1">
       <c r="A205" s="8" t="s">
         <v>391</v>
       </c>
@@ -9928,7 +9929,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="206" spans="1:8">
+    <row r="206" spans="1:8" hidden="1">
       <c r="A206" s="8" t="s">
         <v>391</v>
       </c>
@@ -9954,7 +9955,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="207" spans="1:8">
+    <row r="207" spans="1:8" hidden="1">
       <c r="A207" s="8" t="s">
         <v>391</v>
       </c>
@@ -9980,7 +9981,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="208" spans="1:8">
+    <row r="208" spans="1:8" hidden="1">
       <c r="A208" s="8" t="s">
         <v>391</v>
       </c>
@@ -10006,7 +10007,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="209" spans="1:8">
+    <row r="209" spans="1:8" hidden="1">
       <c r="A209" s="8" t="s">
         <v>391</v>
       </c>
@@ -10032,7 +10033,7 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="210" spans="1:8">
+    <row r="210" spans="1:8" hidden="1">
       <c r="A210" s="8" t="s">
         <v>391</v>
       </c>
@@ -10058,7 +10059,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="211" spans="1:8">
+    <row r="211" spans="1:8" hidden="1">
       <c r="A211" s="8" t="s">
         <v>391</v>
       </c>
@@ -10084,7 +10085,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="212" spans="1:8">
+    <row r="212" spans="1:8" hidden="1">
       <c r="A212" s="8" t="s">
         <v>391</v>
       </c>
@@ -10110,7 +10111,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="213" spans="1:8">
+    <row r="213" spans="1:8" hidden="1">
       <c r="A213" s="8" t="s">
         <v>391</v>
       </c>
@@ -10136,7 +10137,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="214" spans="1:8">
+    <row r="214" spans="1:8" hidden="1">
       <c r="A214" s="8" t="s">
         <v>391</v>
       </c>
@@ -10162,7 +10163,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="215" spans="1:8">
+    <row r="215" spans="1:8" hidden="1">
       <c r="A215" s="8" t="s">
         <v>391</v>
       </c>
@@ -10188,7 +10189,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="216" spans="1:8">
+    <row r="216" spans="1:8" hidden="1">
       <c r="A216" s="8" t="s">
         <v>391</v>
       </c>
@@ -10214,7 +10215,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="217" spans="1:8">
+    <row r="217" spans="1:8" hidden="1">
       <c r="A217" s="8" t="s">
         <v>391</v>
       </c>
@@ -10240,7 +10241,7 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="218" spans="1:8">
+    <row r="218" spans="1:8" hidden="1">
       <c r="A218" s="8" t="s">
         <v>391</v>
       </c>
@@ -10266,7 +10267,7 @@
         <v>1123</v>
       </c>
     </row>
-    <row r="219" spans="1:8">
+    <row r="219" spans="1:8" hidden="1">
       <c r="A219" s="8" t="s">
         <v>391</v>
       </c>
@@ -10293,11 +10294,18 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H219" xr:uid="{0FC232BA-84F4-BE49-B367-4C71587DA4B6}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Quit Tobacco"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D1">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="C16" r:id="rId1" display="https://www.mayoclinic.org/healthy-lifestyle/recipes/chicken-fajitas/rcp-20049943." xr:uid="{BF040B87-8534-9445-90AC-FE2659D40410}"/>

</xml_diff>